<commit_message>
Ya hice lo primero
</commit_message>
<xml_diff>
--- a/Rayos X/Rayos X.xlsx
+++ b/Rayos X/Rayos X.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.laverdeg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\OneDrive\Documentos\Séptimo Semestre\Lab Intermedio\Códigos Bitácoras\Laboratorio-Intermedio\Rayos X\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A596B7-B665-4EAE-AD26-E326060CEEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,18 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="8">
   <si>
     <t>Ángulo del crista</t>
   </si>
   <si>
-    <t>Tasa con 35kV</t>
-  </si>
-  <si>
     <t>theta/°</t>
-  </si>
-  <si>
-    <t>R(35kV)/Imp/s</t>
   </si>
   <si>
     <t>Tasa con 30kV</t>
@@ -50,11 +45,17 @@
   <si>
     <t>Zn</t>
   </si>
+  <si>
+    <t>Ángulo</t>
+  </si>
+  <si>
+    <t>Intensidad</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -365,810 +366,818 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B459"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B457"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2">
         <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3.1</v>
+      </c>
+      <c r="B3">
+        <v>2990</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="B4">
-        <v>3260</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="B5">
-        <v>2990</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="B6">
-        <v>2577</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="B7">
-        <v>2198</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="B8">
-        <v>1911</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3.5</v>
+        <v>3.7</v>
       </c>
       <c r="B9">
-        <v>1634</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="B10">
-        <v>1401</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3.7</v>
+        <v>3.9</v>
       </c>
       <c r="B11">
-        <v>1156</v>
+        <v>991</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>1077</v>
+        <v>933</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3.9</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B13">
-        <v>991</v>
+        <v>950</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="B14">
-        <v>933</v>
+        <v>915</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4.0999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="B15">
-        <v>950</v>
+        <v>914</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B16">
-        <v>915</v>
+        <v>822</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="B17">
-        <v>914</v>
+        <v>822</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>4.4000000000000004</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B18">
-        <v>822</v>
+        <v>783</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
       <c r="B19">
-        <v>822</v>
+        <v>779</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="B20">
-        <v>783</v>
+        <v>725</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="B21">
-        <v>779</v>
+        <v>713</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="B22">
-        <v>725</v>
+        <v>714</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>4.9000000000000004</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B23">
-        <v>713</v>
+        <v>686</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="B24">
-        <v>714</v>
+        <v>666</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>5.0999999999999996</v>
+        <v>5.3</v>
       </c>
       <c r="B25">
-        <v>686</v>
+        <v>636</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>5.2</v>
+        <v>5.4</v>
       </c>
       <c r="B26">
-        <v>666</v>
+        <v>625</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>5.3</v>
+        <v>5.5</v>
       </c>
       <c r="B27">
-        <v>636</v>
+        <v>590</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
       <c r="B28">
-        <v>625</v>
+        <v>596</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>5.5</v>
+        <v>5.7</v>
       </c>
       <c r="B29">
-        <v>590</v>
+        <v>569</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
       <c r="B30">
-        <v>596</v>
+        <v>578</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>5.7</v>
+        <v>5.9</v>
       </c>
       <c r="B31">
-        <v>569</v>
+        <v>554</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="B32">
-        <v>578</v>
+        <v>542</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
       <c r="B33">
-        <v>554</v>
+        <v>558</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>6</v>
+        <v>6.2</v>
       </c>
       <c r="B34">
-        <v>542</v>
+        <v>535</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>6.1</v>
+        <v>6.3</v>
       </c>
       <c r="B35">
-        <v>558</v>
+        <v>541</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>6.2</v>
+        <v>6.4</v>
       </c>
       <c r="B36">
-        <v>535</v>
+        <v>525</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="B37">
-        <v>541</v>
+        <v>512</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>6.4</v>
+        <v>6.6</v>
       </c>
       <c r="B38">
-        <v>525</v>
+        <v>497</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="B39">
-        <v>512</v>
+        <v>486</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>6.6</v>
+        <v>6.8</v>
       </c>
       <c r="B40">
-        <v>497</v>
+        <v>482</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>6.7</v>
+        <v>6.9</v>
       </c>
       <c r="B41">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>6.8</v>
+        <v>7</v>
       </c>
       <c r="B42">
-        <v>482</v>
+        <v>456</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>6.9</v>
+        <v>7.1</v>
       </c>
       <c r="B43">
-        <v>478</v>
+        <v>454</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>7</v>
+        <v>7.2</v>
       </c>
       <c r="B44">
-        <v>456</v>
+        <v>424</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>7.1</v>
+        <v>7.3</v>
       </c>
       <c r="B45">
-        <v>454</v>
+        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>7.2</v>
+        <v>7.4</v>
       </c>
       <c r="B46">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>7.3</v>
+        <v>7.5</v>
       </c>
       <c r="B47">
-        <v>430</v>
+        <v>404</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>7.4</v>
+        <v>7.6</v>
       </c>
       <c r="B48">
-        <v>426</v>
+        <v>417</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>7.5</v>
+        <v>7.7</v>
       </c>
       <c r="B49">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>7.6</v>
+        <v>7.8</v>
       </c>
       <c r="B50">
-        <v>417</v>
+        <v>373</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>7.7</v>
+        <v>7.9</v>
       </c>
       <c r="B51">
-        <v>396</v>
+        <v>361</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>7.8</v>
+        <v>8</v>
       </c>
       <c r="B52">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="B53">
-        <v>361</v>
+        <v>338</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>8</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="B54">
-        <v>377</v>
+        <v>332</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>8.1</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="B55">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>8.1999999999999993</v>
+        <v>8.4</v>
       </c>
       <c r="B56">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>8.3000000000000007</v>
+        <v>8.5</v>
       </c>
       <c r="B57">
-        <v>340</v>
+        <v>322</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>8.4</v>
+        <v>8.6</v>
       </c>
       <c r="B58">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>8.5</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="B59">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>8.6</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="B60">
-        <v>323</v>
+        <v>280</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>8.6999999999999993</v>
+        <v>8.9</v>
       </c>
       <c r="B61">
-        <v>312</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>8.8000000000000007</v>
+        <v>9</v>
       </c>
       <c r="B62">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>8.9</v>
+        <v>9.1</v>
       </c>
       <c r="B63">
-        <v>292</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>9</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="B64">
-        <v>287</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>9.1</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="B65">
-        <v>267</v>
+        <v>275</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>9.1999999999999993</v>
+        <v>9.4</v>
       </c>
       <c r="B66">
-        <v>268</v>
+        <v>255</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>9.3000000000000007</v>
+        <v>9.5</v>
       </c>
       <c r="B67">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>9.4</v>
+        <v>9.6</v>
       </c>
       <c r="B68">
-        <v>255</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>9.5</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="B69">
-        <v>254</v>
+        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>9.6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="B70">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>9.6999999999999993</v>
+        <v>9.9</v>
       </c>
       <c r="B71">
-        <v>240</v>
+        <v>227</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>9.8000000000000007</v>
+        <v>10</v>
       </c>
       <c r="B72">
-        <v>230</v>
+        <v>242</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>9.9</v>
+        <v>10.1</v>
       </c>
       <c r="B73">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>10</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="B74">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>10.1</v>
+        <v>10.3</v>
       </c>
       <c r="B75">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>10.199999999999999</v>
+        <v>10.4</v>
       </c>
       <c r="B76">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>10.3</v>
+        <v>10.5</v>
       </c>
       <c r="B77">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>10.4</v>
+        <v>10.6</v>
       </c>
       <c r="B78">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>10.5</v>
+        <v>10.7</v>
       </c>
       <c r="B79">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>10.6</v>
+        <v>10.8</v>
       </c>
       <c r="B80">
-        <v>226</v>
+        <v>240</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>10.7</v>
+        <v>10.9</v>
       </c>
       <c r="B81">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>10.8</v>
+        <v>11</v>
       </c>
       <c r="B82">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>10.9</v>
+        <v>11.1</v>
       </c>
       <c r="B83">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>11</v>
+        <v>11.2</v>
       </c>
       <c r="B84">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>11.1</v>
+        <v>11.3</v>
       </c>
       <c r="B85">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>11.2</v>
+        <v>11.4</v>
       </c>
       <c r="B86">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>11.3</v>
+        <v>11.5</v>
       </c>
       <c r="B87">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>11.4</v>
+        <v>11.6</v>
       </c>
       <c r="B88">
-        <v>236</v>
+        <v>251</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>11.5</v>
+        <v>11.7</v>
       </c>
       <c r="B89">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>11.6</v>
+        <v>11.8</v>
       </c>
       <c r="B90">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>11.7</v>
+        <v>11.9</v>
       </c>
       <c r="B91">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>11.8</v>
+        <v>12</v>
       </c>
       <c r="B92">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>11.9</v>
+        <v>12.1</v>
       </c>
       <c r="B93">
-        <v>250</v>
+        <v>234</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>12</v>
+        <v>12.2</v>
       </c>
       <c r="B94">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>12.1</v>
+        <v>12.3</v>
       </c>
       <c r="B95">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>12.2</v>
+        <v>12.4</v>
       </c>
       <c r="B96">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>12.3</v>
+        <v>12.5</v>
       </c>
       <c r="B97">
-        <v>233</v>
+        <v>245</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>12.4</v>
+        <v>12.6</v>
       </c>
       <c r="B98">
-        <v>234</v>
+        <v>244</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>12.5</v>
+        <v>12.7</v>
       </c>
       <c r="B99">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>12.6</v>
+        <v>12.8</v>
       </c>
       <c r="B100">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>12.7</v>
+        <v>12.9</v>
       </c>
       <c r="B101">
         <v>249</v>
@@ -1176,519 +1185,519 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>12.8</v>
+        <v>13</v>
       </c>
       <c r="B102">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>12.9</v>
+        <v>13.1</v>
       </c>
       <c r="B103">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>13</v>
+        <v>13.2</v>
       </c>
       <c r="B104">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>13.1</v>
+        <v>13.3</v>
       </c>
       <c r="B105">
-        <v>235</v>
+        <v>247</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>13.2</v>
+        <v>13.4</v>
       </c>
       <c r="B106">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>13.3</v>
+        <v>13.5</v>
       </c>
       <c r="B107">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>13.4</v>
+        <v>13.6</v>
       </c>
       <c r="B108">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>13.5</v>
+        <v>13.7</v>
       </c>
       <c r="B109">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>13.6</v>
+        <v>13.8</v>
       </c>
       <c r="B110">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>13.7</v>
+        <v>13.9</v>
       </c>
       <c r="B111">
-        <v>235</v>
+        <v>247</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>13.8</v>
+        <v>14</v>
       </c>
       <c r="B112">
-        <v>238</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>13.9</v>
+        <v>14.1</v>
       </c>
       <c r="B113">
-        <v>247</v>
+        <v>262</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>14</v>
+        <v>14.2</v>
       </c>
       <c r="B114">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>14.1</v>
+        <v>14.3</v>
       </c>
       <c r="B115">
-        <v>262</v>
+        <v>243</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>14.2</v>
+        <v>14.4</v>
       </c>
       <c r="B116">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>14.3</v>
+        <v>14.5</v>
       </c>
       <c r="B117">
-        <v>243</v>
+        <v>260</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>14.4</v>
+        <v>14.6</v>
       </c>
       <c r="B118">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>14.5</v>
+        <v>14.7</v>
       </c>
       <c r="B119">
-        <v>260</v>
+        <v>240</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>14.6</v>
+        <v>14.8</v>
       </c>
       <c r="B120">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>14.7</v>
+        <v>14.9</v>
       </c>
       <c r="B121">
-        <v>240</v>
+        <v>262</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>14.8</v>
+        <v>15</v>
       </c>
       <c r="B122">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>14.9</v>
+        <v>15.1</v>
       </c>
       <c r="B123">
-        <v>262</v>
+        <v>250</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>15</v>
+        <v>15.2</v>
       </c>
       <c r="B124">
-        <v>248</v>
+        <v>234</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>15.1</v>
+        <v>15.3</v>
       </c>
       <c r="B125">
-        <v>250</v>
+        <v>262</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>15.2</v>
+        <v>15.4</v>
       </c>
       <c r="B126">
-        <v>234</v>
+        <v>244</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>15.3</v>
+        <v>15.5</v>
       </c>
       <c r="B127">
-        <v>262</v>
+        <v>248</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>15.4</v>
+        <v>15.6</v>
       </c>
       <c r="B128">
-        <v>244</v>
+        <v>269</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>15.5</v>
+        <v>15.7</v>
       </c>
       <c r="B129">
-        <v>248</v>
+        <v>282</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>15.6</v>
+        <v>15.8</v>
       </c>
       <c r="B130">
-        <v>269</v>
+        <v>283</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>15.7</v>
+        <v>15.9</v>
       </c>
       <c r="B131">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>15.8</v>
+        <v>16</v>
       </c>
       <c r="B132">
-        <v>283</v>
+        <v>268</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>15.9</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="B133">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>16</v>
+        <v>16.2</v>
       </c>
       <c r="B134">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>16.100000000000001</v>
+        <v>16.3</v>
       </c>
       <c r="B135">
-        <v>271</v>
+        <v>256</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>16.2</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="B136">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>16.3</v>
+        <v>16.5</v>
       </c>
       <c r="B137">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>16.399999999999999</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="B138">
-        <v>267</v>
+        <v>253</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>16.5</v>
+        <v>16.7</v>
       </c>
       <c r="B139">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>16.600000000000001</v>
+        <v>16.8</v>
       </c>
       <c r="B140">
-        <v>253</v>
+        <v>273</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>16.7</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="B141">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>16.8</v>
+        <v>17</v>
       </c>
       <c r="B142">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>16.899999999999999</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="B143">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>17</v>
+        <v>17.2</v>
       </c>
       <c r="B144">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>17.100000000000001</v>
+        <v>17.3</v>
       </c>
       <c r="B145">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>17.2</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="B146">
-        <v>251</v>
+        <v>268</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>17.3</v>
+        <v>17.5</v>
       </c>
       <c r="B147">
-        <v>265</v>
+        <v>272</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>17.399999999999999</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="B148">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>17.5</v>
+        <v>17.7</v>
       </c>
       <c r="B149">
-        <v>272</v>
+        <v>320</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>17.600000000000001</v>
+        <v>17.8</v>
       </c>
       <c r="B150">
-        <v>263</v>
+        <v>350</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>17.7</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="B151">
-        <v>320</v>
+        <v>756</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>17.8</v>
+        <v>18</v>
       </c>
       <c r="B152">
-        <v>350</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>17.899999999999999</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="B153">
-        <v>756</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>18</v>
+        <v>18.2</v>
       </c>
       <c r="B154">
-        <v>1710</v>
+        <v>432</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>18.100000000000001</v>
+        <v>18.3</v>
       </c>
       <c r="B155">
-        <v>1589</v>
+        <v>356</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>18.2</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="B156">
-        <v>432</v>
+        <v>323</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>18.3</v>
+        <v>18.5</v>
       </c>
       <c r="B157">
-        <v>356</v>
+        <v>308</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>18.399999999999999</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="B158">
-        <v>323</v>
+        <v>302</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>18.5</v>
+        <v>18.7</v>
       </c>
       <c r="B159">
-        <v>308</v>
+        <v>290</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>18.600000000000001</v>
+        <v>18.8</v>
       </c>
       <c r="B160">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>18.7</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="B161">
-        <v>290</v>
+        <v>303</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>18.8</v>
+        <v>19</v>
       </c>
       <c r="B162">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>18.899999999999999</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="B163">
-        <v>303</v>
+        <v>311</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>19</v>
+        <v>19.2</v>
       </c>
       <c r="B164">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>19.100000000000001</v>
+        <v>19.3</v>
       </c>
       <c r="B165">
-        <v>311</v>
+        <v>292</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="B166">
         <v>294</v>
@@ -1696,151 +1705,151 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>19.3</v>
+        <v>19.5</v>
       </c>
       <c r="B167">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>19.399999999999999</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="B168">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>19.5</v>
+        <v>19.7</v>
       </c>
       <c r="B169">
-        <v>294</v>
+        <v>340</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>19.600000000000001</v>
+        <v>19.8</v>
       </c>
       <c r="B170">
-        <v>298</v>
+        <v>353</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>19.7</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="B171">
-        <v>340</v>
+        <v>402</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>19.8</v>
+        <v>20</v>
       </c>
       <c r="B172">
-        <v>353</v>
+        <v>481</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>19.899999999999999</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="B173">
-        <v>402</v>
+        <v>818</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>20</v>
+        <v>20.2</v>
       </c>
       <c r="B174">
-        <v>481</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>20.100000000000001</v>
+        <v>20.3</v>
       </c>
       <c r="B175">
-        <v>818</v>
+        <v>7304</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>20.2</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="B176">
-        <v>3800</v>
+        <v>4377</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>20.3</v>
+        <v>20.5</v>
       </c>
       <c r="B177">
-        <v>7304</v>
+        <v>778</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>20.399999999999999</v>
+        <v>20.6</v>
       </c>
       <c r="B178">
-        <v>4377</v>
+        <v>407</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>20.5</v>
+        <v>20.7</v>
       </c>
       <c r="B179">
-        <v>778</v>
+        <v>362</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>20.6</v>
+        <v>20.8</v>
       </c>
       <c r="B180">
-        <v>407</v>
+        <v>306</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>20.7</v>
+        <v>20.9</v>
       </c>
       <c r="B181">
-        <v>362</v>
+        <v>262</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>20.8</v>
+        <v>21</v>
       </c>
       <c r="B182">
-        <v>306</v>
+        <v>269</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>20.9</v>
+        <v>21.1</v>
       </c>
       <c r="B183">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>21</v>
+        <v>21.2</v>
       </c>
       <c r="B184">
-        <v>269</v>
+        <v>249</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>21.1</v>
+        <v>21.3</v>
       </c>
       <c r="B185">
         <v>254</v>
@@ -1848,479 +1857,479 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>21.2</v>
+        <v>21.4</v>
       </c>
       <c r="B186">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>21.3</v>
+        <v>21.5</v>
       </c>
       <c r="B187">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>21.4</v>
+        <v>21.6</v>
       </c>
       <c r="B188">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>21.5</v>
+        <v>21.7</v>
       </c>
       <c r="B189">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>21.6</v>
+        <v>21.8</v>
       </c>
       <c r="B190">
-        <v>245</v>
+        <v>227</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>21.7</v>
+        <v>21.9</v>
       </c>
       <c r="B191">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>21.8</v>
+        <v>22</v>
       </c>
       <c r="B192">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>21.9</v>
+        <v>22.1</v>
       </c>
       <c r="B193">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>22</v>
+        <v>22.2</v>
       </c>
       <c r="B194">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>22.1</v>
+        <v>22.3</v>
       </c>
       <c r="B195">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>22.2</v>
+        <v>22.4</v>
       </c>
       <c r="B196">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>22.3</v>
+        <v>22.5</v>
       </c>
       <c r="B197">
-        <v>236</v>
+        <v>212</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>22.4</v>
+        <v>22.6</v>
       </c>
       <c r="B198">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>22.5</v>
+        <v>22.7</v>
       </c>
       <c r="B199">
-        <v>212</v>
+        <v>224</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>22.6</v>
+        <v>22.8</v>
       </c>
       <c r="B200">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>22.7</v>
+        <v>22.9</v>
       </c>
       <c r="B201">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>22.8</v>
+        <v>23</v>
       </c>
       <c r="B202">
-        <v>209</v>
+        <v>223</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>22.9</v>
+        <v>23.1</v>
       </c>
       <c r="B203">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>23</v>
+        <v>23.2</v>
       </c>
       <c r="B204">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>23.1</v>
+        <v>23.3</v>
       </c>
       <c r="B205">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>23.2</v>
+        <v>23.4</v>
       </c>
       <c r="B206">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>23.3</v>
+        <v>23.5</v>
       </c>
       <c r="B207">
-        <v>206</v>
+        <v>217</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>23.4</v>
+        <v>23.6</v>
       </c>
       <c r="B208">
-        <v>215</v>
+        <v>196</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209">
-        <v>23.5</v>
+        <v>23.7</v>
       </c>
       <c r="B209">
-        <v>217</v>
+        <v>199</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210">
-        <v>23.6</v>
+        <v>23.8</v>
       </c>
       <c r="B210">
-        <v>196</v>
+        <v>207</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>23.7</v>
+        <v>23.9</v>
       </c>
       <c r="B211">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212">
-        <v>23.8</v>
+        <v>24</v>
       </c>
       <c r="B212">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213">
-        <v>23.9</v>
+        <v>24.1</v>
       </c>
       <c r="B213">
-        <v>205</v>
+        <v>227</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>24</v>
+        <v>24.2</v>
       </c>
       <c r="B214">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215">
-        <v>24.1</v>
+        <v>24.3</v>
       </c>
       <c r="B215">
-        <v>227</v>
+        <v>204</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216">
-        <v>24.2</v>
+        <v>24.4</v>
       </c>
       <c r="B216">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217">
-        <v>24.3</v>
+        <v>24.5</v>
       </c>
       <c r="B217">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>24.4</v>
+        <v>24.6</v>
       </c>
       <c r="B218">
-        <v>197</v>
+        <v>220</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>24.5</v>
+        <v>24.7</v>
       </c>
       <c r="B219">
-        <v>187</v>
+        <v>206</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220">
-        <v>24.6</v>
+        <v>24.8</v>
       </c>
       <c r="B220">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221">
-        <v>24.7</v>
+        <v>24.9</v>
       </c>
       <c r="B221">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>24.8</v>
+        <v>25</v>
       </c>
       <c r="B222">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223">
-        <v>24.9</v>
+        <v>25.1</v>
       </c>
       <c r="B223">
-        <v>202</v>
+        <v>211</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224">
-        <v>25</v>
+        <v>25.2</v>
       </c>
       <c r="B224">
-        <v>191</v>
+        <v>215</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
       <c r="B225">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>25.2</v>
+        <v>25.4</v>
       </c>
       <c r="B226">
-        <v>215</v>
+        <v>191</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>25.3</v>
+        <v>25.5</v>
       </c>
       <c r="B227">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>25.4</v>
+        <v>25.6</v>
       </c>
       <c r="B228">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>25.5</v>
+        <v>25.7</v>
       </c>
       <c r="B229">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230">
-        <v>25.6</v>
+        <v>25.8</v>
       </c>
       <c r="B230">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231">
-        <v>25.7</v>
+        <v>25.9</v>
       </c>
       <c r="B231">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>25.8</v>
+        <v>26</v>
       </c>
       <c r="B232">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233">
-        <v>25.9</v>
+        <v>26.1</v>
       </c>
       <c r="B233">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234">
-        <v>26</v>
+        <v>26.2</v>
       </c>
       <c r="B234">
-        <v>196</v>
+        <v>205</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235">
-        <v>26.1</v>
+        <v>26.3</v>
       </c>
       <c r="B235">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>26.2</v>
+        <v>26.4</v>
       </c>
       <c r="B236">
-        <v>205</v>
+        <v>182</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>26.3</v>
+        <v>26.5</v>
       </c>
       <c r="B237">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238">
-        <v>26.4</v>
+        <v>26.6</v>
       </c>
       <c r="B238">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239">
-        <v>26.5</v>
+        <v>26.7</v>
       </c>
       <c r="B239">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240">
-        <v>26.6</v>
+        <v>26.8</v>
       </c>
       <c r="B240">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241">
-        <v>26.7</v>
+        <v>26.9</v>
       </c>
       <c r="B241">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242">
-        <v>26.8</v>
+        <v>27</v>
       </c>
       <c r="B242">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243">
-        <v>26.9</v>
+        <v>27.1</v>
       </c>
       <c r="B243">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244">
-        <v>27</v>
+        <v>27.2</v>
       </c>
       <c r="B244">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>27.1</v>
+        <v>27.3</v>
       </c>
       <c r="B245">
         <v>196</v>
@@ -2328,279 +2337,279 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246">
-        <v>27.2</v>
+        <v>27.4</v>
       </c>
       <c r="B246">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247">
-        <v>27.3</v>
+        <v>27.5</v>
       </c>
       <c r="B247">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248">
-        <v>27.4</v>
+        <v>27.6</v>
       </c>
       <c r="B248">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249">
-        <v>27.5</v>
+        <v>27.7</v>
       </c>
       <c r="B249">
-        <v>185</v>
+        <v>203</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250">
-        <v>27.6</v>
+        <v>27.8</v>
       </c>
       <c r="B250">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251">
-        <v>27.7</v>
+        <v>27.9</v>
       </c>
       <c r="B251">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>27.8</v>
+        <v>28</v>
       </c>
       <c r="B252">
-        <v>202</v>
+        <v>182</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253">
-        <v>27.9</v>
+        <v>28.1</v>
       </c>
       <c r="B253">
-        <v>189</v>
+        <v>205</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254">
-        <v>28</v>
+        <v>28.2</v>
       </c>
       <c r="B254">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255">
-        <v>28.1</v>
+        <v>28.3</v>
       </c>
       <c r="B255">
-        <v>205</v>
+        <v>181</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256">
-        <v>28.2</v>
+        <v>28.4</v>
       </c>
       <c r="B256">
-        <v>175</v>
+        <v>187</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257">
-        <v>28.3</v>
+        <v>28.5</v>
       </c>
       <c r="B257">
-        <v>181</v>
+        <v>196</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258">
-        <v>28.4</v>
+        <v>28.6</v>
       </c>
       <c r="B258">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259">
-        <v>28.5</v>
+        <v>28.7</v>
       </c>
       <c r="B259">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260">
-        <v>28.6</v>
+        <v>28.8</v>
       </c>
       <c r="B260">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261">
-        <v>28.7</v>
+        <v>28.9</v>
       </c>
       <c r="B261">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262">
-        <v>28.8</v>
+        <v>29</v>
       </c>
       <c r="B262">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263">
-        <v>28.9</v>
+        <v>29.1</v>
       </c>
       <c r="B263">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264">
-        <v>29</v>
+        <v>29.2</v>
       </c>
       <c r="B264">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265">
-        <v>29.1</v>
+        <v>29.3</v>
       </c>
       <c r="B265">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266">
-        <v>29.2</v>
+        <v>29.4</v>
       </c>
       <c r="B266">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267">
-        <v>29.3</v>
+        <v>29.5</v>
       </c>
       <c r="B267">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268">
-        <v>29.4</v>
+        <v>29.6</v>
       </c>
       <c r="B268">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269">
-        <v>29.5</v>
+        <v>29.7</v>
       </c>
       <c r="B269">
-        <v>182</v>
+        <v>198</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270">
-        <v>29.6</v>
+        <v>29.8</v>
       </c>
       <c r="B270">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271">
-        <v>29.7</v>
+        <v>29.9</v>
       </c>
       <c r="B271">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272">
-        <v>29.8</v>
+        <v>30</v>
       </c>
       <c r="B272">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273">
-        <v>29.9</v>
+        <v>30.1</v>
       </c>
       <c r="B273">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274">
-        <v>30</v>
+        <v>30.2</v>
       </c>
       <c r="B274">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275">
-        <v>30.1</v>
+        <v>30.3</v>
       </c>
       <c r="B275">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276">
-        <v>30.2</v>
+        <v>30.4</v>
       </c>
       <c r="B276">
-        <v>174</v>
+        <v>186</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277">
-        <v>30.3</v>
+        <v>30.5</v>
       </c>
       <c r="B277">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278">
-        <v>30.4</v>
+        <v>30.6</v>
       </c>
       <c r="B278">
-        <v>186</v>
+        <v>199</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279">
-        <v>30.5</v>
+        <v>30.7</v>
       </c>
       <c r="B279">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280">
-        <v>30.6</v>
+        <v>30.8</v>
       </c>
       <c r="B280">
         <v>199</v>
@@ -2608,295 +2617,295 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281">
-        <v>30.7</v>
+        <v>30.9</v>
       </c>
       <c r="B281">
-        <v>187</v>
+        <v>200</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282">
-        <v>30.8</v>
+        <v>31</v>
       </c>
       <c r="B282">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283">
-        <v>30.9</v>
+        <v>31.1</v>
       </c>
       <c r="B283">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284">
-        <v>31</v>
+        <v>31.2</v>
       </c>
       <c r="B284">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285">
-        <v>31.1</v>
+        <v>31.3</v>
       </c>
       <c r="B285">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286">
-        <v>31.2</v>
+        <v>31.4</v>
       </c>
       <c r="B286">
-        <v>202</v>
+        <v>177</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287">
-        <v>31.3</v>
+        <v>31.5</v>
       </c>
       <c r="B287">
-        <v>185</v>
+        <v>194</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288">
-        <v>31.4</v>
+        <v>31.6</v>
       </c>
       <c r="B288">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289">
-        <v>31.5</v>
+        <v>31.7</v>
       </c>
       <c r="B289">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290">
-        <v>31.6</v>
+        <v>31.8</v>
       </c>
       <c r="B290">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291">
-        <v>31.7</v>
+        <v>31.9</v>
       </c>
       <c r="B291">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292">
-        <v>31.8</v>
+        <v>32</v>
       </c>
       <c r="B292">
-        <v>177</v>
+        <v>201</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293">
-        <v>31.9</v>
+        <v>32.1</v>
       </c>
       <c r="B293">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294">
-        <v>32</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="B294">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295">
-        <v>32.1</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="B295">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296">
-        <v>32.200000000000003</v>
+        <v>32.4</v>
       </c>
       <c r="B296">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297">
-        <v>32.299999999999997</v>
+        <v>32.5</v>
       </c>
       <c r="B297">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298">
-        <v>32.4</v>
+        <v>32.6</v>
       </c>
       <c r="B298">
-        <v>171</v>
+        <v>184</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299">
-        <v>32.5</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="B299">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300">
-        <v>32.6</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="B300">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301">
-        <v>32.700000000000003</v>
+        <v>32.9</v>
       </c>
       <c r="B301">
-        <v>159</v>
+        <v>173</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302">
-        <v>32.799999999999997</v>
+        <v>33</v>
       </c>
       <c r="B302">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303">
-        <v>32.9</v>
+        <v>33.1</v>
       </c>
       <c r="B303">
-        <v>173</v>
+        <v>185</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304">
-        <v>33</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="B304">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305">
-        <v>33.1</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="B305">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306">
-        <v>33.200000000000003</v>
+        <v>33.4</v>
       </c>
       <c r="B306">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307">
-        <v>33.299999999999997</v>
+        <v>33.5</v>
       </c>
       <c r="B307">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308">
-        <v>33.4</v>
+        <v>33.6</v>
       </c>
       <c r="B308">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309">
-        <v>33.5</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="B309">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310">
-        <v>33.6</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="B310">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311">
-        <v>33.700000000000003</v>
+        <v>33.9</v>
       </c>
       <c r="B311">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312">
-        <v>33.799999999999997</v>
+        <v>34</v>
       </c>
       <c r="B312">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313">
-        <v>33.9</v>
+        <v>34.1</v>
       </c>
       <c r="B313">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314">
-        <v>34</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="B314">
-        <v>167</v>
+        <v>185</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315">
-        <v>34.1</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="B315">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316">
-        <v>34.200000000000003</v>
+        <v>34.4</v>
       </c>
       <c r="B316">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317">
-        <v>34.299999999999997</v>
+        <v>34.5</v>
       </c>
       <c r="B317">
         <v>176</v>
@@ -2904,31 +2913,31 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318">
-        <v>34.4</v>
+        <v>34.6</v>
       </c>
       <c r="B318">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319">
-        <v>34.5</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="B319">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320">
-        <v>34.6</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="B320">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321">
-        <v>34.700000000000003</v>
+        <v>34.9</v>
       </c>
       <c r="B321">
         <v>174</v>
@@ -2936,111 +2945,111 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322">
-        <v>34.799999999999997</v>
+        <v>35</v>
       </c>
       <c r="B322">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323">
-        <v>34.9</v>
+        <v>35.1</v>
       </c>
       <c r="B323">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324">
-        <v>35</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="B324">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325">
-        <v>35.1</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="B325">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326">
-        <v>35.200000000000003</v>
+        <v>35.4</v>
       </c>
       <c r="B326">
-        <v>180</v>
+        <v>163</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327">
-        <v>35.299999999999997</v>
+        <v>35.5</v>
       </c>
       <c r="B327">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328">
-        <v>35.4</v>
+        <v>35.6</v>
       </c>
       <c r="B328">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329">
-        <v>35.5</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="B329">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330">
-        <v>35.6</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="B330">
-        <v>173</v>
+        <v>195</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331">
-        <v>35.700000000000003</v>
+        <v>35.9</v>
       </c>
       <c r="B331">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332">
-        <v>35.799999999999997</v>
+        <v>36</v>
       </c>
       <c r="B332">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333">
-        <v>35.9</v>
+        <v>36.1</v>
       </c>
       <c r="B333">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334">
-        <v>36</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="B334">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335">
-        <v>36.1</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="B335">
         <v>168</v>
@@ -3048,95 +3057,95 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336">
-        <v>36.200000000000003</v>
+        <v>36.4</v>
       </c>
       <c r="B336">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337">
-        <v>36.299999999999997</v>
+        <v>36.5</v>
       </c>
       <c r="B337">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338">
-        <v>36.4</v>
+        <v>36.6</v>
       </c>
       <c r="B338">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339">
-        <v>36.5</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="B339">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340">
-        <v>36.6</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="B340">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341">
-        <v>36.700000000000003</v>
+        <v>36.9</v>
       </c>
       <c r="B341">
-        <v>171</v>
+        <v>182</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342">
-        <v>36.799999999999997</v>
+        <v>37</v>
       </c>
       <c r="B342">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343">
-        <v>36.9</v>
+        <v>37.1</v>
       </c>
       <c r="B343">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344">
-        <v>37</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="B344">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345">
-        <v>37.1</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="B345">
-        <v>172</v>
+        <v>185</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346">
-        <v>37.200000000000003</v>
+        <v>37.4</v>
       </c>
       <c r="B346">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347">
-        <v>37.299999999999997</v>
+        <v>37.5</v>
       </c>
       <c r="B347">
         <v>185</v>
@@ -3144,897 +3153,881 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348">
-        <v>37.4</v>
+        <v>37.6</v>
       </c>
       <c r="B348">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349">
-        <v>37.5</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="B349">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350">
-        <v>37.6</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="B350">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351">
-        <v>37.700000000000003</v>
+        <v>37.9</v>
       </c>
       <c r="B351">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352">
-        <v>37.799999999999997</v>
+        <v>38</v>
       </c>
       <c r="B352">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353">
-        <v>37.9</v>
+        <v>38.1</v>
       </c>
       <c r="B353">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354">
-        <v>38</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="B354">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355">
-        <v>38.1</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="B355">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356">
-        <v>38.200000000000003</v>
+        <v>38.4</v>
       </c>
       <c r="B356">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357">
-        <v>38.299999999999997</v>
+        <v>38.5</v>
       </c>
       <c r="B357">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358">
-        <v>38.4</v>
+        <v>38.6</v>
       </c>
       <c r="B358">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359">
-        <v>38.5</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="B359">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360">
-        <v>38.6</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="B360">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361">
-        <v>38.700000000000003</v>
+        <v>38.9</v>
       </c>
       <c r="B361">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362">
-        <v>38.799999999999997</v>
+        <v>39</v>
       </c>
       <c r="B362">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363">
-        <v>38.9</v>
+        <v>39.1</v>
       </c>
       <c r="B363">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364">
-        <v>39</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="B364">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365">
-        <v>39.1</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="B365">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366">
-        <v>39.200000000000003</v>
+        <v>39.4</v>
       </c>
       <c r="B366">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367">
-        <v>39.299999999999997</v>
+        <v>39.5</v>
       </c>
       <c r="B367">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368">
-        <v>39.4</v>
+        <v>39.6</v>
       </c>
       <c r="B368">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369">
-        <v>39.5</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="B369">
-        <v>163</v>
+        <v>180</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370">
-        <v>39.6</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="B370">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371">
-        <v>39.700000000000003</v>
+        <v>39.9</v>
       </c>
       <c r="B371">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372">
-        <v>39.799999999999997</v>
+        <v>40</v>
       </c>
       <c r="B372">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373">
-        <v>39.9</v>
+        <v>40.1</v>
       </c>
       <c r="B373">
-        <v>164</v>
+        <v>187</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374">
-        <v>40</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="B374">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375">
-        <v>40.1</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="B375">
-        <v>187</v>
+        <v>169</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376">
-        <v>40.200000000000003</v>
+        <v>40.4</v>
       </c>
       <c r="B376">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377">
-        <v>40.299999999999997</v>
+        <v>40.5</v>
       </c>
       <c r="B377">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378">
-        <v>40.4</v>
+        <v>40.6</v>
       </c>
       <c r="B378">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379">
-        <v>40.5</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="B379">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380">
-        <v>40.6</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="B380">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381">
-        <v>40.700000000000003</v>
+        <v>40.9</v>
       </c>
       <c r="B381">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382">
-        <v>40.799999999999997</v>
+        <v>41</v>
       </c>
       <c r="B382">
-        <v>180</v>
+        <v>168</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383">
-        <v>40.9</v>
+        <v>41.1</v>
       </c>
       <c r="B383">
-        <v>174</v>
+        <v>193</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384">
-        <v>41</v>
+        <v>41.2</v>
       </c>
       <c r="B384">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385">
-        <v>41.1</v>
+        <v>41.3</v>
       </c>
       <c r="B385">
-        <v>193</v>
+        <v>226</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386">
-        <v>41.2</v>
+        <v>41.4</v>
       </c>
       <c r="B386">
-        <v>184</v>
+        <v>389</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387">
-        <v>41.3</v>
+        <v>41.5</v>
       </c>
       <c r="B387">
-        <v>226</v>
+        <v>446</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388">
-        <v>41.4</v>
+        <v>41.6</v>
       </c>
       <c r="B388">
-        <v>389</v>
+        <v>351</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389">
-        <v>41.5</v>
+        <v>41.7</v>
       </c>
       <c r="B389">
-        <v>446</v>
+        <v>206</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390">
-        <v>41.6</v>
+        <v>41.8</v>
       </c>
       <c r="B390">
-        <v>351</v>
+        <v>170</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391">
-        <v>41.7</v>
+        <v>41.9</v>
       </c>
       <c r="B391">
-        <v>206</v>
+        <v>184</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392">
-        <v>41.8</v>
+        <v>42</v>
       </c>
       <c r="B392">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393">
-        <v>41.9</v>
+        <v>42.1</v>
       </c>
       <c r="B393">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394">
-        <v>42</v>
+        <v>42.2</v>
       </c>
       <c r="B394">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395">
-        <v>42.1</v>
+        <v>42.3</v>
       </c>
       <c r="B395">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396">
-        <v>42.2</v>
+        <v>42.4</v>
       </c>
       <c r="B396">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397">
-        <v>42.3</v>
+        <v>42.5</v>
       </c>
       <c r="B397">
-        <v>172</v>
+        <v>185</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398">
-        <v>42.4</v>
+        <v>42.6</v>
       </c>
       <c r="B398">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399">
-        <v>42.5</v>
+        <v>42.7</v>
       </c>
       <c r="B399">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400">
-        <v>42.6</v>
+        <v>42.8</v>
       </c>
       <c r="B400">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401">
-        <v>42.7</v>
+        <v>42.9</v>
       </c>
       <c r="B401">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402">
-        <v>42.8</v>
+        <v>43</v>
       </c>
       <c r="B402">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403">
-        <v>42.9</v>
+        <v>43.1</v>
       </c>
       <c r="B403">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404">
-        <v>43</v>
+        <v>43.2</v>
       </c>
       <c r="B404">
-        <v>164</v>
+        <v>184</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405">
-        <v>43.1</v>
+        <v>43.3</v>
       </c>
       <c r="B405">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406">
-        <v>43.2</v>
+        <v>43.4</v>
       </c>
       <c r="B406">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407">
-        <v>43.3</v>
+        <v>43.5</v>
       </c>
       <c r="B407">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408">
-        <v>43.4</v>
+        <v>43.6</v>
       </c>
       <c r="B408">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409">
-        <v>43.5</v>
+        <v>43.7</v>
       </c>
       <c r="B409">
-        <v>164</v>
+        <v>185</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410">
-        <v>43.6</v>
+        <v>43.8</v>
       </c>
       <c r="B410">
-        <v>163</v>
+        <v>172</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411">
-        <v>43.7</v>
+        <v>43.9</v>
       </c>
       <c r="B411">
-        <v>185</v>
+        <v>160</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412">
-        <v>43.8</v>
+        <v>44</v>
       </c>
       <c r="B412">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413">
-        <v>43.9</v>
+        <v>44.1</v>
       </c>
       <c r="B413">
-        <v>160</v>
+        <v>172</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414">
-        <v>44</v>
+        <v>44.2</v>
       </c>
       <c r="B414">
-        <v>176</v>
+        <v>155</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415">
-        <v>44.1</v>
+        <v>44.3</v>
       </c>
       <c r="B415">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416">
-        <v>44.2</v>
+        <v>44.4</v>
       </c>
       <c r="B416">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417">
-        <v>44.3</v>
+        <v>44.5</v>
       </c>
       <c r="B417">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418">
-        <v>44.4</v>
+        <v>44.6</v>
       </c>
       <c r="B418">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419">
-        <v>44.5</v>
+        <v>44.7</v>
       </c>
       <c r="B419">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420">
-        <v>44.6</v>
+        <v>44.8</v>
       </c>
       <c r="B420">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421">
-        <v>44.7</v>
+        <v>44.9</v>
       </c>
       <c r="B421">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422">
-        <v>44.8</v>
+        <v>45</v>
       </c>
       <c r="B422">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423">
-        <v>44.9</v>
+        <v>45.1</v>
       </c>
       <c r="B423">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424">
-        <v>45</v>
+        <v>45.2</v>
       </c>
       <c r="B424">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425">
-        <v>45.1</v>
+        <v>45.3</v>
       </c>
       <c r="B425">
-        <v>167</v>
+        <v>182</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426">
-        <v>45.2</v>
+        <v>45.4</v>
       </c>
       <c r="B426">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427">
-        <v>45.3</v>
+        <v>45.5</v>
       </c>
       <c r="B427">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428">
-        <v>45.4</v>
+        <v>45.6</v>
       </c>
       <c r="B428">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429">
-        <v>45.5</v>
+        <v>45.7</v>
       </c>
       <c r="B429">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430">
-        <v>45.6</v>
+        <v>45.8</v>
       </c>
       <c r="B430">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431">
-        <v>45.7</v>
+        <v>45.9</v>
       </c>
       <c r="B431">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432">
-        <v>45.8</v>
+        <v>46</v>
       </c>
       <c r="B432">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433">
-        <v>45.9</v>
+        <v>46.1</v>
       </c>
       <c r="B433">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434">
-        <v>46</v>
+        <v>46.2</v>
       </c>
       <c r="B434">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435">
-        <v>46.1</v>
+        <v>46.3</v>
       </c>
       <c r="B435">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436">
-        <v>46.2</v>
+        <v>46.4</v>
       </c>
       <c r="B436">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437">
-        <v>46.3</v>
+        <v>46.5</v>
       </c>
       <c r="B437">
-        <v>177</v>
+        <v>186</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438">
-        <v>46.4</v>
+        <v>46.6</v>
       </c>
       <c r="B438">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439">
-        <v>46.5</v>
+        <v>46.7</v>
       </c>
       <c r="B439">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440">
-        <v>46.6</v>
+        <v>46.8</v>
       </c>
       <c r="B440">
-        <v>0</v>
+        <v>184</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441">
-        <v>46.7</v>
+        <v>46.9</v>
       </c>
       <c r="B441">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442">
-        <v>46.8</v>
+        <v>47</v>
       </c>
       <c r="B442">
-        <v>184</v>
+        <v>201</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443">
-        <v>46.9</v>
+        <v>47.1</v>
       </c>
       <c r="B443">
-        <v>191</v>
+        <v>202</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444">
-        <v>47</v>
+        <v>47.2</v>
       </c>
       <c r="B444">
-        <v>201</v>
+        <v>226</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445">
-        <v>47.1</v>
+        <v>47.3</v>
       </c>
       <c r="B445">
-        <v>202</v>
+        <v>225</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446">
-        <v>47.2</v>
+        <v>47.4</v>
       </c>
       <c r="B446">
-        <v>226</v>
+        <v>246</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447">
-        <v>47.3</v>
+        <v>47.5</v>
       </c>
       <c r="B447">
-        <v>225</v>
+        <v>419</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448">
-        <v>47.4</v>
+        <v>47.6</v>
       </c>
       <c r="B448">
-        <v>246</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449">
-        <v>47.5</v>
+        <v>47.7</v>
       </c>
       <c r="B449">
-        <v>419</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450">
-        <v>47.6</v>
+        <v>47.8</v>
       </c>
       <c r="B450">
-        <v>1039</v>
+        <v>946</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451">
-        <v>47.7</v>
+        <v>47.9</v>
       </c>
       <c r="B451">
-        <v>1469</v>
+        <v>738</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452">
-        <v>47.8</v>
+        <v>48</v>
       </c>
       <c r="B452">
-        <v>946</v>
+        <v>267</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453">
-        <v>47.9</v>
+        <v>48.1</v>
       </c>
       <c r="B453">
-        <v>738</v>
+        <v>219</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454">
-        <v>48</v>
+        <v>48.2</v>
       </c>
       <c r="B454">
-        <v>267</v>
+        <v>205</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455">
-        <v>48.1</v>
+        <v>48.3</v>
       </c>
       <c r="B455">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456">
-        <v>48.2</v>
+        <v>48.4</v>
       </c>
       <c r="B456">
-        <v>205</v>
+        <v>0</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457">
-        <v>48.3</v>
+        <v>48.5</v>
       </c>
       <c r="B457">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A458">
-        <v>48.4</v>
-      </c>
-      <c r="B458">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A459">
-        <v>48.5</v>
-      </c>
-      <c r="B459">
         <v>211</v>
       </c>
     </row>
@@ -4044,7 +4037,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
@@ -4061,55 +4054,55 @@
         <v>0.02</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G1">
         <v>0.04</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J1">
         <v>0.06</v>
       </c>
       <c r="K1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M1">
         <v>0.08</v>
       </c>
       <c r="N1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P1">
         <v>0.1</v>
       </c>
       <c r="Q1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S1">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="T1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="V1">
         <v>0.05</v>
       </c>
       <c r="W1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Y1">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="Z1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AB1">
         <v>0.1</v>
       </c>
       <c r="AC1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -4117,123 +4110,123 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J2" t="s">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M2" t="s">
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P2" t="s">
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S2" t="s">
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V2" t="s">
         <v>0</v>
       </c>
       <c r="W2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y2" t="s">
         <v>0</v>
       </c>
       <c r="Z2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB2" t="s">
         <v>0</v>
       </c>
       <c r="AC2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Y3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AB3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">

</xml_diff>